<commit_message>
Added Data Cleansing Notebook
</commit_message>
<xml_diff>
--- a/input/sharepoint_list_data.xlsx
+++ b/input/sharepoint_list_data.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1540" windowWidth="27760" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="10360" yWindow="9700" windowWidth="27760" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -66,6 +67,60 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Notes_1</t>
+  </si>
+  <si>
+    <t>Notes_2</t>
+  </si>
+  <si>
+    <t>Company 001</t>
+  </si>
+  <si>
+    <t>Company 002</t>
+  </si>
+  <si>
+    <t>Company 003</t>
+  </si>
+  <si>
+    <t>Company 004</t>
+  </si>
+  <si>
+    <t>Company 005</t>
+  </si>
+  <si>
+    <t>Company 006</t>
+  </si>
+  <si>
+    <t>Company 007</t>
+  </si>
+  <si>
+    <t>Company 008</t>
+  </si>
+  <si>
+    <t>Company 009</t>
+  </si>
+  <si>
+    <t>Company 010</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
   </si>
 </sst>
 </file>
@@ -382,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -461,4 +516,346 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.87001607940156156</v>
+      </c>
+      <c r="G2">
+        <v>0.18366716439731878</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>9.238234628081321E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.11574112636337619</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.27007960504501938</v>
+      </c>
+      <c r="G4">
+        <v>0.19845950723333794</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.59801876806207455</v>
+      </c>
+      <c r="G5">
+        <v>0.58131423496351209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.17695636781258961</v>
+      </c>
+      <c r="G6">
+        <v>0.35726218281172617</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.93497349335220259</v>
+      </c>
+      <c r="G7">
+        <v>0.86843209899135509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>7.7893863321325973E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.31234413831136498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0.27333504899498684</v>
+      </c>
+      <c r="G9">
+        <v>0.51202917172740459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.700316980058725</v>
+      </c>
+      <c r="G10">
+        <v>0.468006308488357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.700316980058725</v>
+      </c>
+      <c r="G11">
+        <v>0.468006308488357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.2591384043226258</v>
+      </c>
+      <c r="G12">
+        <v>0.5554633890754721</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0.2591384043226258</v>
+      </c>
+      <c r="G13">
+        <v>0.5554633890754721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0.2591384043226258</v>
+      </c>
+      <c r="G14">
+        <v>0.5554633890754721</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>